<commit_message>
TobaccoUse en reparaties aan Drug en AlcoholUSe
</commit_message>
<xml_diff>
--- a/maps/SubstanceUse-AlcoholUse.xlsx
+++ b/maps/SubstanceUse-AlcoholUse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_C233CE142FFFD580DB94AA4299532E306390057D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42CAF809-E433-AD4C-A476-714C17AFBFF6}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_C233CE142FFFD580DB94AA4299532E306390057D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE2CC7A7-CCCA-BE4D-8A21-0B25CCB9C138}"/>
   <bookViews>
     <workbookView xWindow="26620" yWindow="620" windowWidth="24340" windowHeight="13420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,7 +355,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -433,9 +433,6 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -453,6 +450,9 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>